<commit_message>
upload and department view backend added
</commit_message>
<xml_diff>
--- a/media/ranks.xlsx
+++ b/media/ranks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VSC\Projects\Student Ranking System\Student-Ranking-System\media\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anshu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CA3647-7227-40F8-BCC4-F0261FFACAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9669C3E7-385A-41C8-A0D4-103662E99B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{89F90A9E-4853-4D04-898D-50F6C9BB12F1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
   <si>
     <t>STUDENT NAME</t>
   </si>
@@ -103,6 +103,135 @@
   </si>
   <si>
     <t>BCA</t>
+  </si>
+  <si>
+    <t>JATIN SAHU</t>
+  </si>
+  <si>
+    <t>SHREEYA PANIGRAHI</t>
+  </si>
+  <si>
+    <t>ARPITA PADHAN</t>
+  </si>
+  <si>
+    <t>MANISKA SAHU</t>
+  </si>
+  <si>
+    <t>POOJA SAHU</t>
+  </si>
+  <si>
+    <t>ABANI KARTI</t>
+  </si>
+  <si>
+    <t>ARPITA HOTA</t>
+  </si>
+  <si>
+    <t>LINGARAJ BEHERA</t>
+  </si>
+  <si>
+    <t>OMKAR SAHU</t>
+  </si>
+  <si>
+    <t>ADARSHA NANDA</t>
+  </si>
+  <si>
+    <t>ABHINAV BAGARTY</t>
+  </si>
+  <si>
+    <t>DEBASMITH PRADHAN</t>
+  </si>
+  <si>
+    <t>SHIBANANDA SAHOO</t>
+  </si>
+  <si>
+    <t>PRIYANKA SAHOO</t>
+  </si>
+  <si>
+    <t>SHRIYARANI HOTA</t>
+  </si>
+  <si>
+    <t>SRUSTIMAYEE SAHU</t>
+  </si>
+  <si>
+    <t>SWAGAT PUROHIT</t>
+  </si>
+  <si>
+    <t>PRATYUSHNA MISHRA</t>
+  </si>
+  <si>
+    <t>SUBHRANKITA TRIPATHY</t>
+  </si>
+  <si>
+    <t>ELIZA NAYAK</t>
+  </si>
+  <si>
+    <t>CHANDRAKANTA BHOI</t>
+  </si>
+  <si>
+    <t>SNEHA SINGH</t>
+  </si>
+  <si>
+    <t>SUBHADARSHINI HOTA</t>
+  </si>
+  <si>
+    <t>MADHUSMITA PRADHAN</t>
+  </si>
+  <si>
+    <t>NIHAR SATAPATHY</t>
+  </si>
+  <si>
+    <t>NIHARIKA BEHERA</t>
+  </si>
+  <si>
+    <t>PRAKRUTI PASAYAT</t>
+  </si>
+  <si>
+    <t>SHIKHA SAI</t>
+  </si>
+  <si>
+    <t>SMRUTI MISHRA</t>
+  </si>
+  <si>
+    <t>BIDYUT SAHU</t>
+  </si>
+  <si>
+    <t>LALITENDU SAHOO</t>
+  </si>
+  <si>
+    <t>ANWESHA MAHAKUR</t>
+  </si>
+  <si>
+    <t>BINAYA BHOI</t>
+  </si>
+  <si>
+    <t>RASESWARI SAHU</t>
+  </si>
+  <si>
+    <t>SMITA KUMAR</t>
+  </si>
+  <si>
+    <t>MOLISKA PATTNAIK</t>
+  </si>
+  <si>
+    <t>ANISHA BHOI</t>
+  </si>
+  <si>
+    <t>BSC(CHE)</t>
+  </si>
+  <si>
+    <t>BSC(MAT)</t>
+  </si>
+  <si>
+    <t>BSC(PHY)</t>
+  </si>
+  <si>
+    <t>BSC(IT)</t>
+  </si>
+  <si>
+    <t>BSC(BOT)</t>
+  </si>
+  <si>
+    <t>BSC(ZOO)</t>
   </si>
 </sst>
 </file>
@@ -158,7 +287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -167,9 +296,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -493,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FAAE10B-68ED-4100-BD41-802DF28D3D5A}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,27 +636,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
+      <c r="A2" s="5">
         <v>210614100001</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -543,14 +669,14 @@
         <v>6</v>
       </c>
       <c r="E2" s="2">
-        <v>8.5299999999999994</v>
-      </c>
-      <c r="F2" s="2">
-        <v>9.1</v>
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="F2" s="1">
+        <v>9.5299999999999994</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>210614100002</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -563,14 +689,14 @@
         <v>6</v>
       </c>
       <c r="E3" s="2">
-        <v>8.5399999999999991</v>
-      </c>
-      <c r="F3" s="2">
-        <v>9.11</v>
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="F3" s="1">
+        <v>8.7200000000000006</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>210614100003</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -583,14 +709,14 @@
         <v>6</v>
       </c>
       <c r="E4" s="2">
-        <v>8.5500000000000007</v>
-      </c>
-      <c r="F4" s="2">
-        <v>9.1199999999999992</v>
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="F4" s="1">
+        <v>9.2899999999999991</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>210614100004</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -603,14 +729,14 @@
         <v>6</v>
       </c>
       <c r="E5" s="2">
-        <v>8.56</v>
-      </c>
-      <c r="F5" s="2">
-        <v>9.1300000000000008</v>
+        <v>9.1</v>
+      </c>
+      <c r="F5" s="1">
+        <v>8.9499999999999993</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="6">
+      <c r="A6" s="5">
         <v>210614100005</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -623,14 +749,14 @@
         <v>6</v>
       </c>
       <c r="E6" s="2">
-        <v>8.57</v>
-      </c>
-      <c r="F6" s="2">
-        <v>9.14</v>
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="F6" s="1">
+        <v>9.52</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="6">
+      <c r="A7" s="5">
         <v>210614100007</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -643,14 +769,14 @@
         <v>6</v>
       </c>
       <c r="E7" s="2">
-        <v>8.58</v>
-      </c>
-      <c r="F7" s="2">
-        <v>9.15</v>
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="F7" s="1">
+        <v>8.98</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>210614100008</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -663,14 +789,14 @@
         <v>6</v>
       </c>
       <c r="E8" s="2">
-        <v>8.59</v>
-      </c>
-      <c r="F8" s="2">
-        <v>9.16</v>
+        <v>8.67</v>
+      </c>
+      <c r="F8" s="1">
+        <v>9.5500000000000007</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>210614100009</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -683,14 +809,14 @@
         <v>6</v>
       </c>
       <c r="E9" s="2">
-        <v>8.6</v>
-      </c>
-      <c r="F9" s="2">
-        <v>9.17</v>
+        <v>9.24</v>
+      </c>
+      <c r="F9" s="1">
+        <v>8.61</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="6">
+      <c r="A10" s="5">
         <v>210614100010</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -703,14 +829,14 @@
         <v>6</v>
       </c>
       <c r="E10" s="2">
-        <v>8.61</v>
-      </c>
-      <c r="F10" s="2">
+        <v>8.65</v>
+      </c>
+      <c r="F10" s="1">
         <v>9.18</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
+      <c r="A11" s="5">
         <v>210614100011</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -723,14 +849,14 @@
         <v>6</v>
       </c>
       <c r="E11" s="2">
-        <v>8.6199999999999992</v>
-      </c>
-      <c r="F11" s="2">
-        <v>9.19</v>
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="F11" s="1">
+        <v>9.0299999999999994</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="6">
+      <c r="A12" s="5">
         <v>210614100012</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -743,14 +869,14 @@
         <v>6</v>
       </c>
       <c r="E12" s="2">
-        <v>8.6300000000000008</v>
-      </c>
-      <c r="F12" s="2">
-        <v>9.1999999999999993</v>
+        <v>8.93</v>
+      </c>
+      <c r="F12" s="1">
+        <v>9.6</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
+      <c r="A13" s="5">
         <v>210614100013</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -763,14 +889,14 @@
         <v>6</v>
       </c>
       <c r="E13" s="2">
-        <v>8.64</v>
-      </c>
-      <c r="F13" s="2">
-        <v>9.2100000000000009</v>
+        <v>9.5</v>
+      </c>
+      <c r="F13" s="1">
+        <v>8.66</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="6">
+      <c r="A14" s="5">
         <v>210614100014</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -783,14 +909,14 @@
         <v>6</v>
       </c>
       <c r="E14" s="2">
-        <v>8.65</v>
-      </c>
-      <c r="F14" s="2">
-        <v>9.2200000000000006</v>
+        <v>8.83</v>
+      </c>
+      <c r="F14" s="1">
+        <v>9.23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
+      <c r="A15" s="5">
         <v>210614100015</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -803,14 +929,14 @@
         <v>6</v>
       </c>
       <c r="E15" s="2">
-        <v>8.66</v>
-      </c>
-      <c r="F15" s="2">
-        <v>9.23</v>
+        <v>9.4</v>
+      </c>
+      <c r="F15" s="1">
+        <v>8.74</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="6">
+      <c r="A16" s="5">
         <v>210614100016</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -823,14 +949,14 @@
         <v>6</v>
       </c>
       <c r="E16" s="2">
-        <v>8.67</v>
-      </c>
-      <c r="F16" s="2">
-        <v>9.24</v>
+        <v>8.5500000000000007</v>
+      </c>
+      <c r="F16" s="1">
+        <v>9.31</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
+      <c r="A17" s="5">
         <v>210614100017</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -843,14 +969,751 @@
         <v>6</v>
       </c>
       <c r="E17" s="2">
+        <v>9.1199999999999992</v>
+      </c>
+      <c r="F17" s="1">
+        <v>8.57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="5">
+        <v>210604100001</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="1">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2">
+        <v>8.9</v>
+      </c>
+      <c r="F18" s="1">
+        <v>9.14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>210604100002</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="1">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2">
+        <v>9.4700000000000006</v>
+      </c>
+      <c r="F19" s="1">
+        <v>8.69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>210604100003</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="1">
+        <v>6</v>
+      </c>
+      <c r="E20" s="2">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="F20" s="1">
+        <v>9.26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>210604110002</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="1">
+        <v>6</v>
+      </c>
+      <c r="E21" s="2">
+        <v>9.6199999999999992</v>
+      </c>
+      <c r="F21" s="1">
+        <v>8.64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>210604110003</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="1">
+        <v>6</v>
+      </c>
+      <c r="E22" s="2">
+        <v>8.59</v>
+      </c>
+      <c r="F22" s="1">
+        <v>9.2100000000000009</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>210604120001</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="1">
+        <v>6</v>
+      </c>
+      <c r="E23" s="2">
+        <v>9.16</v>
+      </c>
+      <c r="F23" s="1">
+        <v>8.6199999999999992</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
+        <v>210604120002</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D24" s="1">
+        <v>6</v>
+      </c>
+      <c r="E24" s="2">
+        <v>8.7799999999999994</v>
+      </c>
+      <c r="F24" s="1">
+        <v>9.19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
+        <v>210604120003</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="1">
+        <v>6</v>
+      </c>
+      <c r="E25" s="2">
+        <v>9.35</v>
+      </c>
+      <c r="F25" s="1">
+        <v>8.8699999999999992</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>210604120004</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="1">
+        <v>6</v>
+      </c>
+      <c r="E26" s="2">
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="F26" s="1">
+        <v>9.44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>210604140001</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="1">
+        <v>6</v>
+      </c>
+      <c r="E27" s="2">
+        <v>9.4499999999999993</v>
+      </c>
+      <c r="F27" s="1">
+        <v>8.58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>210604140002</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="1">
+        <v>6</v>
+      </c>
+      <c r="E28" s="2">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="F28" s="1">
+        <v>9.15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
+        <v>210604140004</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" s="1">
+        <v>6</v>
+      </c>
+      <c r="E29" s="2">
+        <v>9.27</v>
+      </c>
+      <c r="F29" s="1">
+        <v>8.73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
+        <v>210604140005</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="1">
+        <v>6</v>
+      </c>
+      <c r="E30" s="2">
+        <v>8.91</v>
+      </c>
+      <c r="F30" s="1">
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>210604160001</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="1">
+        <v>6</v>
+      </c>
+      <c r="E31" s="2">
+        <v>9.48</v>
+      </c>
+      <c r="F31" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>210604160002</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="1">
+        <v>6</v>
+      </c>
+      <c r="E32" s="2">
+        <v>8.77</v>
+      </c>
+      <c r="F32" s="1">
+        <v>9.3699999999999992</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>210604160003</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="1">
+        <v>6</v>
+      </c>
+      <c r="E33" s="2">
+        <v>9.34</v>
+      </c>
+      <c r="F33" s="1">
+        <v>9.02</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
+        <v>210604160004</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="1">
+        <v>6</v>
+      </c>
+      <c r="E34" s="2">
+        <v>8.56</v>
+      </c>
+      <c r="F34" s="1">
+        <v>9.59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
+        <v>210604160005</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="1">
+        <v>6</v>
+      </c>
+      <c r="E35" s="2">
+        <v>9.1300000000000008</v>
+      </c>
+      <c r="F35" s="1">
+        <v>8.94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
+        <v>210604160006</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="1">
+        <v>6</v>
+      </c>
+      <c r="E36" s="2">
+        <v>8.92</v>
+      </c>
+      <c r="F36" s="1">
+        <v>9.51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="5">
+        <v>210604160007</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="1">
+        <v>6</v>
+      </c>
+      <c r="E37" s="2">
+        <v>9.49</v>
+      </c>
+      <c r="F37" s="1">
+        <v>8.7899999999999991</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="5">
+        <v>210604160008</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D38" s="1">
+        <v>6</v>
+      </c>
+      <c r="E38" s="2">
+        <v>8.5399999999999991</v>
+      </c>
+      <c r="F38" s="1">
+        <v>9.36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="5">
+        <v>210604170001</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="1">
+        <v>6</v>
+      </c>
+      <c r="E39" s="2">
+        <v>9.11</v>
+      </c>
+      <c r="F39" s="1">
+        <v>8.86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="5">
+        <v>210604170003</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D40" s="1">
+        <v>6</v>
+      </c>
+      <c r="E40" s="2">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="F40" s="1">
+        <v>9.43</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="5">
+        <v>210604170004</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D41" s="1">
+        <v>6</v>
+      </c>
+      <c r="E41" s="2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="F41" s="1">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="5">
+        <v>210604170005</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42" s="1">
+        <v>6</v>
+      </c>
+      <c r="E42" s="2">
+        <v>9</v>
+      </c>
+      <c r="F42" s="1">
+        <v>9.17</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="5">
+        <v>210604170006</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43" s="1">
+        <v>6</v>
+      </c>
+      <c r="E43" s="2">
+        <v>9.57</v>
+      </c>
+      <c r="F43" s="1">
+        <v>8.99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="5">
+        <v>210604170007</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" s="1">
+        <v>6</v>
+      </c>
+      <c r="E44" s="2">
+        <v>8.85</v>
+      </c>
+      <c r="F44" s="1">
+        <v>9.56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="5">
+        <v>210604170008</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" s="1">
+        <v>6</v>
+      </c>
+      <c r="E45" s="2">
+        <v>9.42</v>
+      </c>
+      <c r="F45" s="1">
+        <v>8.76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="5">
+        <v>210604170009</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D46" s="1">
+        <v>6</v>
+      </c>
+      <c r="E46" s="2">
+        <v>9.01</v>
+      </c>
+      <c r="F46" s="1">
+        <v>9.33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="5">
+        <v>210604170010</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" s="1">
+        <v>6</v>
+      </c>
+      <c r="E47" s="2">
+        <v>9.58</v>
+      </c>
+      <c r="F47" s="1">
+        <v>8.84</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="5">
+        <v>210604170011</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D48" s="1">
+        <v>6</v>
+      </c>
+      <c r="E48" s="2">
         <v>8.68</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F48" s="1">
+        <v>9.41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="5">
+        <v>210604170012</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" s="1">
+        <v>6</v>
+      </c>
+      <c r="E49" s="2">
         <v>9.25</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
+      <c r="F49" s="1">
+        <v>9.0399999999999991</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="5">
+        <v>210604170013</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" s="1">
+        <v>6</v>
+      </c>
+      <c r="E50" s="2">
+        <v>8.82</v>
+      </c>
+      <c r="F50" s="1">
+        <v>9.61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="5">
+        <v>210604170014</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D51" s="1">
+        <v>6</v>
+      </c>
+      <c r="E51" s="2">
+        <v>9.39</v>
+      </c>
+      <c r="F51" s="1">
+        <v>8.9700000000000006</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="5">
+        <v>210604170015</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D52" s="1">
+        <v>6</v>
+      </c>
+      <c r="E52" s="2">
+        <v>8.89</v>
+      </c>
+      <c r="F52" s="1">
+        <v>9.5399999999999991</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="5">
+        <v>210604170016</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D53" s="1">
+        <v>6</v>
+      </c>
+      <c r="E53" s="2">
+        <v>9.4600000000000009</v>
+      </c>
+      <c r="F53" s="1">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="5">
+        <v>210604170017</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D54" s="1">
+        <v>6</v>
+      </c>
+      <c r="E54" s="2">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="F54" s="1">
+        <v>9.32</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>